<commit_message>
modfied data for ML
</commit_message>
<xml_diff>
--- a/Data Collection/UK City Data.xlsx
+++ b/Data Collection/UK City Data.xlsx
@@ -13,13 +13,14 @@
   </bookViews>
   <sheets>
     <sheet name="data-tool-export" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="547">
   <si>
     <t>City</t>
   </si>
@@ -1661,6 +1662,9 @@
   <si>
     <t>Data generated from: http://www.centreforcities.org/data-tool/su/0f2917be</t>
   </si>
+  <si>
+    <t>Uber In</t>
+  </si>
 </sst>
 </file>
 
@@ -2471,11 +2475,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:OR123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="HM1" workbookViewId="0">
-      <selection activeCell="IB5" sqref="IB5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="69" max="69" width="10.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -81250,7 +81257,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>528</v>
       </c>
@@ -81282,7 +81289,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>534</v>
       </c>
@@ -81298,7 +81305,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>538</v>
       </c>
@@ -81333,6 +81340,4187 @@
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>545</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U64"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>546</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" t="s">
+        <v>150</v>
+      </c>
+      <c r="L1" t="s">
+        <v>167</v>
+      </c>
+      <c r="M1" t="s">
+        <v>186</v>
+      </c>
+      <c r="N1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O1" t="s">
+        <v>218</v>
+      </c>
+      <c r="P1" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>272</v>
+      </c>
+      <c r="R1" t="s">
+        <v>274</v>
+      </c>
+      <c r="S1" t="s">
+        <v>276</v>
+      </c>
+      <c r="T1" t="s">
+        <v>278</v>
+      </c>
+      <c r="U1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>593.4</v>
+      </c>
+      <c r="D2">
+        <v>45.789930599999998</v>
+      </c>
+      <c r="E2">
+        <v>47.309027800000003</v>
+      </c>
+      <c r="F2">
+        <v>6.1501099999999997</v>
+      </c>
+      <c r="G2">
+        <v>1.835379718</v>
+      </c>
+      <c r="H2">
+        <v>12.944065480000001</v>
+      </c>
+      <c r="I2">
+        <v>59.155979989999999</v>
+      </c>
+      <c r="J2">
+        <v>15.42701228</v>
+      </c>
+      <c r="K2">
+        <v>75.8</v>
+      </c>
+      <c r="L2">
+        <v>62771.659885300003</v>
+      </c>
+      <c r="M2">
+        <v>7.4303197650000001</v>
+      </c>
+      <c r="N2">
+        <v>114234</v>
+      </c>
+      <c r="O2">
+        <v>202731.81659239999</v>
+      </c>
+      <c r="P2">
+        <v>230400</v>
+      </c>
+      <c r="Q2">
+        <v>20.098028209999999</v>
+      </c>
+      <c r="R2">
+        <v>19.93913633</v>
+      </c>
+      <c r="S2">
+        <v>20.920765020000001</v>
+      </c>
+      <c r="T2">
+        <v>24.665047820000002</v>
+      </c>
+      <c r="U2">
+        <v>14.37702262</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>566</v>
+      </c>
+      <c r="D3">
+        <v>41.984732800000003</v>
+      </c>
+      <c r="E3">
+        <v>63.794983600000002</v>
+      </c>
+      <c r="F3">
+        <v>5.5974785999999996</v>
+      </c>
+      <c r="G3">
+        <v>2.2664098689999999</v>
+      </c>
+      <c r="H3">
+        <v>9.2707303109999994</v>
+      </c>
+      <c r="I3">
+        <v>68.907396800000001</v>
+      </c>
+      <c r="J3">
+        <v>7.7767945449999996</v>
+      </c>
+      <c r="K3">
+        <v>83.8</v>
+      </c>
+      <c r="L3">
+        <v>66967.228275899994</v>
+      </c>
+      <c r="M3">
+        <v>11.56262433</v>
+      </c>
+      <c r="N3">
+        <v>73940</v>
+      </c>
+      <c r="O3">
+        <v>360379.76406449999</v>
+      </c>
+      <c r="P3">
+        <v>183400</v>
+      </c>
+      <c r="Q3">
+        <v>24.811198600000001</v>
+      </c>
+      <c r="R3">
+        <v>12.64344183</v>
+      </c>
+      <c r="S3">
+        <v>22.720073800000002</v>
+      </c>
+      <c r="T3">
+        <v>25.46081989</v>
+      </c>
+      <c r="U3">
+        <v>14.364465879999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>411</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>451.5</v>
+      </c>
+      <c r="D4">
+        <v>24.655244499999998</v>
+      </c>
+      <c r="E4">
+        <v>36.356038400000003</v>
+      </c>
+      <c r="F4">
+        <v>5.6580668000000003</v>
+      </c>
+      <c r="G4">
+        <v>0.68739802500000002</v>
+      </c>
+      <c r="H4">
+        <v>8.3211847960000007</v>
+      </c>
+      <c r="I4">
+        <v>73.595999190000001</v>
+      </c>
+      <c r="J4">
+        <v>9.3648326399999995</v>
+      </c>
+      <c r="K4">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="L4">
+        <v>43126.898978500001</v>
+      </c>
+      <c r="M4">
+        <v>5.2325785649999998</v>
+      </c>
+      <c r="N4">
+        <v>107830</v>
+      </c>
+      <c r="O4">
+        <v>123857.22767009999</v>
+      </c>
+      <c r="P4">
+        <v>239300</v>
+      </c>
+      <c r="Q4">
+        <v>23.478403780000001</v>
+      </c>
+      <c r="R4">
+        <v>12.1005445</v>
+      </c>
+      <c r="S4">
+        <v>19.775452919999999</v>
+      </c>
+      <c r="T4">
+        <v>27.341807190000001</v>
+      </c>
+      <c r="U4">
+        <v>17.303791610000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>412</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>518.20000000000005</v>
+      </c>
+      <c r="D5">
+        <v>41.001651099999997</v>
+      </c>
+      <c r="E5">
+        <v>66.042927899999995</v>
+      </c>
+      <c r="F5">
+        <v>4.6503345999999999</v>
+      </c>
+      <c r="G5">
+        <v>1.70108185</v>
+      </c>
+      <c r="H5">
+        <v>20.164807360000001</v>
+      </c>
+      <c r="I5">
+        <v>61.640122400000003</v>
+      </c>
+      <c r="J5">
+        <v>8.2861479889999998</v>
+      </c>
+      <c r="K5">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="L5">
+        <v>57103.881477700001</v>
+      </c>
+      <c r="M5">
+        <v>10.109694709999999</v>
+      </c>
+      <c r="N5">
+        <v>76120</v>
+      </c>
+      <c r="O5">
+        <v>301386.17492189998</v>
+      </c>
+      <c r="P5">
+        <v>181700</v>
+      </c>
+      <c r="Q5">
+        <v>25.214760139999999</v>
+      </c>
+      <c r="R5">
+        <v>12.048917749999999</v>
+      </c>
+      <c r="S5">
+        <v>21.0318802</v>
+      </c>
+      <c r="T5">
+        <v>25.722505259999998</v>
+      </c>
+      <c r="U5">
+        <v>15.98193665</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>413</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>504</v>
+      </c>
+      <c r="D6">
+        <v>16.697975400000001</v>
+      </c>
+      <c r="E6">
+        <v>32.561051999999997</v>
+      </c>
+      <c r="F6">
+        <v>6.0171625999999998</v>
+      </c>
+      <c r="G6">
+        <v>1.6627557580000001</v>
+      </c>
+      <c r="H6">
+        <v>11.896242340000001</v>
+      </c>
+      <c r="I6">
+        <v>66.143914379999998</v>
+      </c>
+      <c r="J6">
+        <v>11.740690799999999</v>
+      </c>
+      <c r="K6">
+        <v>68.001999999999995</v>
+      </c>
+      <c r="L6">
+        <f>AVERAGE(L7:L64,L2:L5)</f>
+        <v>50926.462292756449</v>
+      </c>
+      <c r="M6">
+        <f>AVERAGE(M7:M64,M2:M5)</f>
+        <v>8.0639970742258047</v>
+      </c>
+      <c r="N6">
+        <v>212402</v>
+      </c>
+      <c r="O6">
+        <f>AVERAGE(O2:O5,O7:O64)</f>
+        <v>211820.01550190005</v>
+      </c>
+      <c r="P6">
+        <v>479100</v>
+      </c>
+      <c r="Q6">
+        <v>25.44617599</v>
+      </c>
+      <c r="R6">
+        <v>15.67353945</v>
+      </c>
+      <c r="S6">
+        <v>20.53039377</v>
+      </c>
+      <c r="T6">
+        <v>23.54020014</v>
+      </c>
+      <c r="U6">
+        <v>14.80969065</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>414</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>428.1</v>
+      </c>
+      <c r="D7">
+        <v>29.1368027</v>
+      </c>
+      <c r="E7">
+        <v>40.978498000000002</v>
+      </c>
+      <c r="F7">
+        <v>4.176069</v>
+      </c>
+      <c r="G7">
+        <v>1.6258245250000001</v>
+      </c>
+      <c r="H7">
+        <v>13.959222179999999</v>
+      </c>
+      <c r="I7">
+        <v>67.329145499999996</v>
+      </c>
+      <c r="J7">
+        <v>7.9990566640000003</v>
+      </c>
+      <c r="K7">
+        <v>69.7</v>
+      </c>
+      <c r="L7">
+        <v>45270.887157899997</v>
+      </c>
+      <c r="M7">
+        <v>6.5381203159999997</v>
+      </c>
+      <c r="N7">
+        <v>146810</v>
+      </c>
+      <c r="O7">
+        <v>169991.12822519999</v>
+      </c>
+      <c r="P7">
+        <v>320900</v>
+      </c>
+      <c r="Q7">
+        <v>23.471854350000001</v>
+      </c>
+      <c r="R7">
+        <v>11.260135780000001</v>
+      </c>
+      <c r="S7">
+        <v>18.447509719999999</v>
+      </c>
+      <c r="T7">
+        <v>27.755696830000002</v>
+      </c>
+      <c r="U7">
+        <v>19.064803319999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>415</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>506.7</v>
+      </c>
+      <c r="D8">
+        <v>32.7345069</v>
+      </c>
+      <c r="E8">
+        <v>54.6780805</v>
+      </c>
+      <c r="F8">
+        <v>4.6907306000000002</v>
+      </c>
+      <c r="G8">
+        <v>1.5300144529999999</v>
+      </c>
+      <c r="H8">
+        <v>17.03802683</v>
+      </c>
+      <c r="I8">
+        <v>64.829591980000004</v>
+      </c>
+      <c r="J8">
+        <v>8.5713521030000006</v>
+      </c>
+      <c r="K8">
+        <v>64.2</v>
+      </c>
+      <c r="L8">
+        <v>48504.976529699998</v>
+      </c>
+      <c r="M8">
+        <v>7.2364270380000004</v>
+      </c>
+      <c r="N8">
+        <v>1007070</v>
+      </c>
+      <c r="O8">
+        <v>177602.56393569999</v>
+      </c>
+      <c r="P8">
+        <v>2488200</v>
+      </c>
+      <c r="Q8">
+        <v>26.899318040000001</v>
+      </c>
+      <c r="R8">
+        <v>14.61620169</v>
+      </c>
+      <c r="S8">
+        <v>20.31626369</v>
+      </c>
+      <c r="T8">
+        <v>22.905104359999999</v>
+      </c>
+      <c r="U8">
+        <v>15.263112209999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>416</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>481.4</v>
+      </c>
+      <c r="D9">
+        <v>32.016348800000003</v>
+      </c>
+      <c r="E9">
+        <v>47.343324299999999</v>
+      </c>
+      <c r="F9">
+        <v>4.7626137999999996</v>
+      </c>
+      <c r="G9">
+        <v>0.978140542</v>
+      </c>
+      <c r="H9">
+        <v>7.0022966479999997</v>
+      </c>
+      <c r="I9">
+        <v>71.093633830000002</v>
+      </c>
+      <c r="J9">
+        <v>12.325892639999999</v>
+      </c>
+      <c r="K9">
+        <v>65.3</v>
+      </c>
+      <c r="L9">
+        <v>41527.024556700002</v>
+      </c>
+      <c r="M9">
+        <v>5.468320254</v>
+      </c>
+      <c r="N9">
+        <v>60290</v>
+      </c>
+      <c r="O9">
+        <v>118717.2327138</v>
+      </c>
+      <c r="P9">
+        <v>146800</v>
+      </c>
+      <c r="Q9">
+        <v>28.67739289</v>
+      </c>
+      <c r="R9">
+        <v>14.01392646</v>
+      </c>
+      <c r="S9">
+        <v>20.924950339999999</v>
+      </c>
+      <c r="T9">
+        <v>23.46005465</v>
+      </c>
+      <c r="U9">
+        <v>12.923675660000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>417</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>502.8</v>
+      </c>
+      <c r="D10">
+        <v>36.191793500000003</v>
+      </c>
+      <c r="E10">
+        <v>45.182111599999999</v>
+      </c>
+      <c r="F10">
+        <v>5.2149251000000003</v>
+      </c>
+      <c r="G10">
+        <v>2.9970082040000001</v>
+      </c>
+      <c r="H10">
+        <v>7.8318339610000001</v>
+      </c>
+      <c r="I10">
+        <v>65.388985599999998</v>
+      </c>
+      <c r="J10">
+        <v>12.54052476</v>
+      </c>
+      <c r="K10">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="L10">
+        <v>41303.747903399999</v>
+      </c>
+      <c r="M10">
+        <v>6.4451507010000002</v>
+      </c>
+      <c r="N10">
+        <v>107540</v>
+      </c>
+      <c r="O10">
+        <v>146394.33889079999</v>
+      </c>
+      <c r="P10">
+        <v>216900</v>
+      </c>
+      <c r="Q10">
+        <v>21.870150859999999</v>
+      </c>
+      <c r="R10">
+        <v>11.06086621</v>
+      </c>
+      <c r="S10">
+        <v>18.286490799999999</v>
+      </c>
+      <c r="T10">
+        <v>27.856231229999999</v>
+      </c>
+      <c r="U10">
+        <v>20.926260889999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>418</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>480.5</v>
+      </c>
+      <c r="D11">
+        <v>38.7243736</v>
+      </c>
+      <c r="E11">
+        <v>53.9449161</v>
+      </c>
+      <c r="F11">
+        <v>4.2579756</v>
+      </c>
+      <c r="G11">
+        <v>4.2929589689999998</v>
+      </c>
+      <c r="H11">
+        <v>7.3637489489999997</v>
+      </c>
+      <c r="I11">
+        <v>67.00143731</v>
+      </c>
+      <c r="J11">
+        <v>9.5382515389999991</v>
+      </c>
+      <c r="K11">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="L11">
+        <v>51098.082557200003</v>
+      </c>
+      <c r="M11">
+        <v>12.498758560000001</v>
+      </c>
+      <c r="N11">
+        <v>218290</v>
+      </c>
+      <c r="O11">
+        <v>309274.9806368</v>
+      </c>
+      <c r="P11">
+        <v>482800</v>
+      </c>
+      <c r="Q11">
+        <v>20.869899199999999</v>
+      </c>
+      <c r="R11">
+        <v>12.7768456</v>
+      </c>
+      <c r="S11">
+        <v>19.000802480000001</v>
+      </c>
+      <c r="T11">
+        <v>25.68650843</v>
+      </c>
+      <c r="U11">
+        <v>21.665944289999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>419</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>467.5</v>
+      </c>
+      <c r="D12">
+        <v>29.555722899999999</v>
+      </c>
+      <c r="E12">
+        <v>44.145331300000002</v>
+      </c>
+      <c r="F12">
+        <v>4.5086987000000001</v>
+      </c>
+      <c r="G12">
+        <v>0.76780078299999999</v>
+      </c>
+      <c r="H12">
+        <v>14.051987560000001</v>
+      </c>
+      <c r="I12">
+        <v>65.284990660000005</v>
+      </c>
+      <c r="J12">
+        <v>10.585236849999999</v>
+      </c>
+      <c r="K12">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="L12">
+        <v>47861.973802799999</v>
+      </c>
+      <c r="M12">
+        <v>6.302195974</v>
+      </c>
+      <c r="N12">
+        <v>210730</v>
+      </c>
+      <c r="O12">
+        <v>152059.3844639</v>
+      </c>
+      <c r="P12">
+        <v>531200</v>
+      </c>
+      <c r="Q12">
+        <v>28.76532198</v>
+      </c>
+      <c r="R12">
+        <v>14.25757773</v>
+      </c>
+      <c r="S12">
+        <v>20.75578235</v>
+      </c>
+      <c r="T12">
+        <v>22.939332230000002</v>
+      </c>
+      <c r="U12">
+        <v>13.281985710000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>420</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>471.2</v>
+      </c>
+      <c r="D13">
+        <v>47.175222300000001</v>
+      </c>
+      <c r="E13">
+        <v>69.544020599999996</v>
+      </c>
+      <c r="F13">
+        <v>3.7873819000000002</v>
+      </c>
+      <c r="G13">
+        <v>4.5691250099999996</v>
+      </c>
+      <c r="H13">
+        <v>21.586603539999999</v>
+      </c>
+      <c r="I13">
+        <v>43.846458480000003</v>
+      </c>
+      <c r="J13">
+        <v>17.453111790000001</v>
+      </c>
+      <c r="K13">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="L13">
+        <v>52468.574353099997</v>
+      </c>
+      <c r="M13">
+        <v>13.706271470000001</v>
+      </c>
+      <c r="N13">
+        <v>154310</v>
+      </c>
+      <c r="O13">
+        <v>367902.78701189999</v>
+      </c>
+      <c r="P13">
+        <v>348700</v>
+      </c>
+      <c r="Q13">
+        <v>21.85526273</v>
+      </c>
+      <c r="R13">
+        <v>17.109499</v>
+      </c>
+      <c r="S13">
+        <v>23.163882340000001</v>
+      </c>
+      <c r="T13">
+        <v>23.187197170000001</v>
+      </c>
+      <c r="U13">
+        <v>14.68415877</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>421</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>525.20000000000005</v>
+      </c>
+      <c r="D14">
+        <v>37.707182299999999</v>
+      </c>
+      <c r="E14">
+        <v>56.629834299999999</v>
+      </c>
+      <c r="F14">
+        <v>5.2497188000000001</v>
+      </c>
+      <c r="G14">
+        <v>6.07515742</v>
+      </c>
+      <c r="H14">
+        <v>9.3482162950000003</v>
+      </c>
+      <c r="I14">
+        <v>61.208394179999999</v>
+      </c>
+      <c r="J14">
+        <v>14.1458361</v>
+      </c>
+      <c r="K14">
+        <v>77.3</v>
+      </c>
+      <c r="L14">
+        <v>54873.461317000001</v>
+      </c>
+      <c r="M14">
+        <v>10.3839044</v>
+      </c>
+      <c r="N14">
+        <v>307850</v>
+      </c>
+      <c r="O14">
+        <v>275947.92945559998</v>
+      </c>
+      <c r="P14">
+        <v>724000</v>
+      </c>
+      <c r="Q14">
+        <v>23.907924879999999</v>
+      </c>
+      <c r="R14">
+        <v>16.814302730000001</v>
+      </c>
+      <c r="S14">
+        <v>21.582313190000001</v>
+      </c>
+      <c r="T14">
+        <v>23.183034469999999</v>
+      </c>
+      <c r="U14">
+        <v>14.512424729999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>422</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>457.9</v>
+      </c>
+      <c r="D15">
+        <v>27.323943700000001</v>
+      </c>
+      <c r="E15">
+        <v>37.183098600000001</v>
+      </c>
+      <c r="F15">
+        <v>4.9881869999999999</v>
+      </c>
+      <c r="G15">
+        <v>1.1554798150000001</v>
+      </c>
+      <c r="H15">
+        <v>7.5215926260000003</v>
+      </c>
+      <c r="I15">
+        <v>70.609499459999995</v>
+      </c>
+      <c r="J15">
+        <v>12.128019419999999</v>
+      </c>
+      <c r="K15">
+        <v>74</v>
+      </c>
+      <c r="L15">
+        <v>45465.783227799999</v>
+      </c>
+      <c r="M15">
+        <v>4.0993107709999999</v>
+      </c>
+      <c r="N15">
+        <v>79710</v>
+      </c>
+      <c r="O15">
+        <v>102596.8647303</v>
+      </c>
+      <c r="P15">
+        <v>177500</v>
+      </c>
+      <c r="Q15">
+        <v>25.076624120000002</v>
+      </c>
+      <c r="R15">
+        <v>13.227504229999999</v>
+      </c>
+      <c r="S15">
+        <v>19.491136529999999</v>
+      </c>
+      <c r="T15">
+        <v>26.067497209999999</v>
+      </c>
+      <c r="U15">
+        <v>16.13723791</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>423</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>602.79999999999995</v>
+      </c>
+      <c r="D16">
+        <v>37.4331551</v>
+      </c>
+      <c r="E16">
+        <v>53.857906800000002</v>
+      </c>
+      <c r="F16">
+        <v>4.7791642999999997</v>
+      </c>
+      <c r="G16">
+        <v>29.034103340000001</v>
+      </c>
+      <c r="H16">
+        <v>11.25561519</v>
+      </c>
+      <c r="I16">
+        <v>33.960327739999997</v>
+      </c>
+      <c r="J16">
+        <v>14.55827178</v>
+      </c>
+      <c r="K16">
+        <v>76.5</v>
+      </c>
+      <c r="L16">
+        <v>59241.735979199999</v>
+      </c>
+      <c r="M16">
+        <v>15.83096712</v>
+      </c>
+      <c r="N16">
+        <v>51120</v>
+      </c>
+      <c r="O16">
+        <v>475815.54781800002</v>
+      </c>
+      <c r="P16">
+        <v>130900</v>
+      </c>
+      <c r="Q16">
+        <v>21.813719549999998</v>
+      </c>
+      <c r="R16">
+        <v>25.363494719999998</v>
+      </c>
+      <c r="S16">
+        <v>22.206883189999999</v>
+      </c>
+      <c r="T16">
+        <v>18.828259339999999</v>
+      </c>
+      <c r="U16">
+        <v>11.7876432</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>424</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>515.5</v>
+      </c>
+      <c r="D17">
+        <v>33.454647299999998</v>
+      </c>
+      <c r="E17">
+        <v>50.391937300000002</v>
+      </c>
+      <c r="F17">
+        <v>5.5317841000000003</v>
+      </c>
+      <c r="G17">
+        <v>3.628127858</v>
+      </c>
+      <c r="H17">
+        <v>13.36975453</v>
+      </c>
+      <c r="I17">
+        <v>60.207751199999997</v>
+      </c>
+      <c r="J17">
+        <v>14.81323693</v>
+      </c>
+      <c r="K17">
+        <v>69.2</v>
+      </c>
+      <c r="L17">
+        <v>44781.0819797</v>
+      </c>
+      <c r="M17">
+        <v>7.8957608700000002</v>
+      </c>
+      <c r="N17">
+        <v>149962</v>
+      </c>
+      <c r="O17">
+        <v>211776.939759</v>
+      </c>
+      <c r="P17">
+        <v>357200</v>
+      </c>
+      <c r="Q17">
+        <v>24.521367269999999</v>
+      </c>
+      <c r="R17">
+        <v>20.009246149999999</v>
+      </c>
+      <c r="S17">
+        <v>20.210349910000001</v>
+      </c>
+      <c r="T17">
+        <v>22.097142359999999</v>
+      </c>
+      <c r="U17">
+        <v>13.1618943</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>425</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>472.5</v>
+      </c>
+      <c r="D18">
+        <v>30.560578700000001</v>
+      </c>
+      <c r="E18">
+        <v>49.547920400000002</v>
+      </c>
+      <c r="F18">
+        <v>3.6307504000000002</v>
+      </c>
+      <c r="G18">
+        <v>1.120065673</v>
+      </c>
+      <c r="H18">
+        <v>13.462100100000001</v>
+      </c>
+      <c r="I18">
+        <v>67.987749530000002</v>
+      </c>
+      <c r="J18">
+        <v>9.1902217240000006</v>
+      </c>
+      <c r="K18">
+        <v>72.3</v>
+      </c>
+      <c r="L18">
+        <v>54148.688639400003</v>
+      </c>
+      <c r="M18">
+        <v>8.2142161439999999</v>
+      </c>
+      <c r="N18">
+        <v>112620</v>
+      </c>
+      <c r="O18">
+        <v>228775.7766639</v>
+      </c>
+      <c r="P18">
+        <v>276500</v>
+      </c>
+      <c r="Q18">
+        <v>26.138865209999999</v>
+      </c>
+      <c r="R18">
+        <v>13.87591172</v>
+      </c>
+      <c r="S18">
+        <v>20.581983520000001</v>
+      </c>
+      <c r="T18">
+        <v>25.382210860000001</v>
+      </c>
+      <c r="U18">
+        <v>14.0210287</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>426</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>518.70000000000005</v>
+      </c>
+      <c r="D19">
+        <v>30.254777099999998</v>
+      </c>
+      <c r="E19">
+        <v>53.995367700000003</v>
+      </c>
+      <c r="F19">
+        <v>4.6003848999999999</v>
+      </c>
+      <c r="G19">
+        <v>2.612678104</v>
+      </c>
+      <c r="H19">
+        <v>13.01686537</v>
+      </c>
+      <c r="I19">
+        <v>65.630997379999997</v>
+      </c>
+      <c r="J19">
+        <v>10.934864790000001</v>
+      </c>
+      <c r="K19">
+        <v>66.3</v>
+      </c>
+      <c r="L19">
+        <v>48971.001234700001</v>
+      </c>
+      <c r="M19">
+        <v>6.7458724060000002</v>
+      </c>
+      <c r="N19">
+        <v>136980</v>
+      </c>
+      <c r="O19">
+        <v>172586.39963170001</v>
+      </c>
+      <c r="P19">
+        <v>345400</v>
+      </c>
+      <c r="Q19">
+        <v>26.170810199999998</v>
+      </c>
+      <c r="R19">
+        <v>17.496845029999999</v>
+      </c>
+      <c r="S19">
+        <v>20.057420489999998</v>
+      </c>
+      <c r="T19">
+        <v>21.683177690000001</v>
+      </c>
+      <c r="U19">
+        <v>14.59174659</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>427</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>634.20000000000005</v>
+      </c>
+      <c r="D20">
+        <v>33.814247100000003</v>
+      </c>
+      <c r="E20">
+        <v>54.102795299999997</v>
+      </c>
+      <c r="F20">
+        <v>5.3618519999999998</v>
+      </c>
+      <c r="G20">
+        <v>2.4952222979999998</v>
+      </c>
+      <c r="H20">
+        <v>18.584357990000001</v>
+      </c>
+      <c r="I20">
+        <v>63.626365700000001</v>
+      </c>
+      <c r="J20">
+        <v>8.2699311289999997</v>
+      </c>
+      <c r="K20">
+        <v>84.9</v>
+      </c>
+      <c r="L20">
+        <v>59485.157699399999</v>
+      </c>
+      <c r="M20">
+        <v>10.165643279999999</v>
+      </c>
+      <c r="N20">
+        <v>44130</v>
+      </c>
+      <c r="O20">
+        <v>283706.83903249999</v>
+      </c>
+      <c r="P20">
+        <v>110900</v>
+      </c>
+      <c r="Q20">
+        <v>25.34780529</v>
+      </c>
+      <c r="R20">
+        <v>14.878467499999999</v>
+      </c>
+      <c r="S20">
+        <v>23.801795550000001</v>
+      </c>
+      <c r="T20">
+        <v>23.337429759999999</v>
+      </c>
+      <c r="U20">
+        <v>12.634501909999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>428</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>578.5</v>
+      </c>
+      <c r="D21">
+        <v>32.245379499999999</v>
+      </c>
+      <c r="E21">
+        <v>45.615414899999998</v>
+      </c>
+      <c r="F21">
+        <v>4.9467806999999997</v>
+      </c>
+      <c r="G21">
+        <v>3.6985643380000002</v>
+      </c>
+      <c r="H21">
+        <v>10.013164679999999</v>
+      </c>
+      <c r="I21">
+        <v>66.655103089999997</v>
+      </c>
+      <c r="J21">
+        <v>12.235149699999999</v>
+      </c>
+      <c r="K21">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="L21">
+        <v>54690.335305699999</v>
+      </c>
+      <c r="M21">
+        <v>5.8686505310000001</v>
+      </c>
+      <c r="N21">
+        <v>108020</v>
+      </c>
+      <c r="O21">
+        <v>158444.1745084</v>
+      </c>
+      <c r="P21">
+        <v>254300</v>
+      </c>
+      <c r="Q21">
+        <v>25.853460470000002</v>
+      </c>
+      <c r="R21">
+        <v>15.388820989999999</v>
+      </c>
+      <c r="S21">
+        <v>20.622145750000001</v>
+      </c>
+      <c r="T21">
+        <v>22.992377950000002</v>
+      </c>
+      <c r="U21">
+        <v>15.143194830000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>429</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>440.2</v>
+      </c>
+      <c r="D22">
+        <v>29.691600999999999</v>
+      </c>
+      <c r="E22">
+        <v>70.045931800000005</v>
+      </c>
+      <c r="F22">
+        <v>7.1082263000000001</v>
+      </c>
+      <c r="G22">
+        <v>2.4115383179999998</v>
+      </c>
+      <c r="H22">
+        <v>9.641669469</v>
+      </c>
+      <c r="I22">
+        <v>70.177483839999994</v>
+      </c>
+      <c r="J22">
+        <v>9.1275268090000008</v>
+      </c>
+      <c r="K22">
+        <v>71.8</v>
+      </c>
+      <c r="L22">
+        <v>43126.898978500001</v>
+      </c>
+      <c r="M22">
+        <v>5.8704236319999996</v>
+      </c>
+      <c r="N22">
+        <v>133040</v>
+      </c>
+      <c r="O22">
+        <v>135963.7076462</v>
+      </c>
+      <c r="P22">
+        <v>304800</v>
+      </c>
+      <c r="Q22">
+        <v>24.019682410000001</v>
+      </c>
+      <c r="R22">
+        <v>13.11366988</v>
+      </c>
+      <c r="S22">
+        <v>19.265084229999999</v>
+      </c>
+      <c r="T22">
+        <v>26.68996898</v>
+      </c>
+      <c r="U22">
+        <v>16.9115945</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>430</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>477.8</v>
+      </c>
+      <c r="D23">
+        <v>26.990553299999998</v>
+      </c>
+      <c r="E23">
+        <v>32.388663999999999</v>
+      </c>
+      <c r="F23">
+        <v>5.1095670999999996</v>
+      </c>
+      <c r="G23">
+        <v>1.2644253160000001</v>
+      </c>
+      <c r="H23">
+        <v>15.354228839999999</v>
+      </c>
+      <c r="I23">
+        <v>60.547515140000002</v>
+      </c>
+      <c r="J23">
+        <v>13.29802832</v>
+      </c>
+      <c r="K23">
+        <v>63.5</v>
+      </c>
+      <c r="L23">
+        <v>47321.713011400003</v>
+      </c>
+      <c r="M23">
+        <v>5.6545009369999999</v>
+      </c>
+      <c r="N23">
+        <v>73689</v>
+      </c>
+      <c r="O23">
+        <v>130492.310832</v>
+      </c>
+      <c r="P23">
+        <v>148200</v>
+      </c>
+      <c r="Q23">
+        <v>22.29404894</v>
+      </c>
+      <c r="R23">
+        <v>18.381454219999998</v>
+      </c>
+      <c r="S23">
+        <v>17.77303963</v>
+      </c>
+      <c r="T23">
+        <v>24.849254420000001</v>
+      </c>
+      <c r="U23">
+        <v>16.702202790000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>431</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>578.20000000000005</v>
+      </c>
+      <c r="D24">
+        <v>41.499599000000003</v>
+      </c>
+      <c r="E24">
+        <v>61.246992800000001</v>
+      </c>
+      <c r="F24">
+        <v>5.1713570999999998</v>
+      </c>
+      <c r="G24">
+        <v>4.2950428919999997</v>
+      </c>
+      <c r="H24">
+        <v>27.607364740000001</v>
+      </c>
+      <c r="I24">
+        <v>40.699134010000002</v>
+      </c>
+      <c r="J24">
+        <v>16.340467570000001</v>
+      </c>
+      <c r="K24">
+        <v>70.8</v>
+      </c>
+      <c r="L24">
+        <v>56883.4286173</v>
+      </c>
+      <c r="M24">
+        <v>7.7369297259999996</v>
+      </c>
+      <c r="N24">
+        <v>241433</v>
+      </c>
+      <c r="O24">
+        <v>234069.97715570001</v>
+      </c>
+      <c r="P24">
+        <v>498800</v>
+      </c>
+      <c r="Q24">
+        <v>20.193610920000001</v>
+      </c>
+      <c r="R24">
+        <v>19.542786169999999</v>
+      </c>
+      <c r="S24">
+        <v>22.115663009999999</v>
+      </c>
+      <c r="T24">
+        <v>23.778811900000001</v>
+      </c>
+      <c r="U24">
+        <v>14.369128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>432</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>520.79999999999995</v>
+      </c>
+      <c r="D25">
+        <v>31.4218382</v>
+      </c>
+      <c r="E25">
+        <v>41.633935600000001</v>
+      </c>
+      <c r="F25">
+        <v>4.3480958999999997</v>
+      </c>
+      <c r="G25">
+        <v>6.1989184269999997</v>
+      </c>
+      <c r="H25">
+        <v>11.0607466</v>
+      </c>
+      <c r="I25">
+        <v>51.850749929999999</v>
+      </c>
+      <c r="J25">
+        <v>22.08824096</v>
+      </c>
+      <c r="K25">
+        <v>76</v>
+      </c>
+      <c r="L25">
+        <v>48677.417670700001</v>
+      </c>
+      <c r="M25">
+        <v>10.51876231</v>
+      </c>
+      <c r="N25">
+        <v>52830</v>
+      </c>
+      <c r="O25">
+        <v>253468.51156069999</v>
+      </c>
+      <c r="P25">
+        <v>127300</v>
+      </c>
+      <c r="Q25">
+        <v>22.93140193</v>
+      </c>
+      <c r="R25">
+        <v>19.683628680000002</v>
+      </c>
+      <c r="S25">
+        <v>19.530792290000001</v>
+      </c>
+      <c r="T25">
+        <v>22.342132750000001</v>
+      </c>
+      <c r="U25">
+        <v>15.512044360000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>433</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>525.20000000000005</v>
+      </c>
+      <c r="D26">
+        <v>34.767536700000001</v>
+      </c>
+      <c r="E26">
+        <v>47.053425799999999</v>
+      </c>
+      <c r="F26">
+        <v>5.0874082999999999</v>
+      </c>
+      <c r="G26">
+        <v>1.3069519030000001</v>
+      </c>
+      <c r="H26">
+        <v>23.12027397</v>
+      </c>
+      <c r="I26">
+        <v>55.933610770000001</v>
+      </c>
+      <c r="J26">
+        <v>9.2808325190000005</v>
+      </c>
+      <c r="K26">
+        <v>69.2</v>
+      </c>
+      <c r="L26">
+        <v>47890.810852399998</v>
+      </c>
+      <c r="M26">
+        <v>5.6023357880000004</v>
+      </c>
+      <c r="N26">
+        <v>472749</v>
+      </c>
+      <c r="O26">
+        <v>154325.52598239999</v>
+      </c>
+      <c r="P26">
+        <v>980800</v>
+      </c>
+      <c r="Q26">
+        <v>22.316506409999999</v>
+      </c>
+      <c r="R26">
+        <v>15.80259672</v>
+      </c>
+      <c r="S26">
+        <v>20.603619389999999</v>
+      </c>
+      <c r="T26">
+        <v>25.884121759999999</v>
+      </c>
+      <c r="U26">
+        <v>15.393155719999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>434</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>535.1</v>
+      </c>
+      <c r="D27">
+        <v>27.908805000000001</v>
+      </c>
+      <c r="E27">
+        <v>42.452830200000001</v>
+      </c>
+      <c r="F27">
+        <v>4.1633262000000002</v>
+      </c>
+      <c r="G27">
+        <v>4.9450907549999998</v>
+      </c>
+      <c r="H27">
+        <v>8.0750806530000006</v>
+      </c>
+      <c r="I27">
+        <v>68.617003940000004</v>
+      </c>
+      <c r="J27">
+        <v>10.877570309999999</v>
+      </c>
+      <c r="K27">
+        <v>80.7</v>
+      </c>
+      <c r="L27">
+        <v>55170.674231500001</v>
+      </c>
+      <c r="M27">
+        <v>7.6363556790000002</v>
+      </c>
+      <c r="N27">
+        <v>54780</v>
+      </c>
+      <c r="O27">
+        <v>187148.7504283</v>
+      </c>
+      <c r="P27">
+        <v>127200</v>
+      </c>
+      <c r="Q27">
+        <v>25.08792979</v>
+      </c>
+      <c r="R27">
+        <v>14.070409570000001</v>
+      </c>
+      <c r="S27">
+        <v>21.048090200000001</v>
+      </c>
+      <c r="T27">
+        <v>24.94822826</v>
+      </c>
+      <c r="U27">
+        <v>14.84534219</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>435</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>421.3</v>
+      </c>
+      <c r="D28">
+        <v>34.653465300000001</v>
+      </c>
+      <c r="E28">
+        <v>47.547778000000001</v>
+      </c>
+      <c r="F28">
+        <v>5.0257977</v>
+      </c>
+      <c r="G28">
+        <v>0.93088769599999999</v>
+      </c>
+      <c r="H28">
+        <v>10.56253476</v>
+      </c>
+      <c r="I28">
+        <v>69.662208870000001</v>
+      </c>
+      <c r="J28">
+        <v>9.2527430259999992</v>
+      </c>
+      <c r="K28">
+        <v>70</v>
+      </c>
+      <c r="L28">
+        <v>44984.3936455</v>
+      </c>
+      <c r="M28">
+        <v>6.7296122059999997</v>
+      </c>
+      <c r="N28">
+        <v>184190</v>
+      </c>
+      <c r="O28">
+        <v>163036.96898899999</v>
+      </c>
+      <c r="P28">
+        <v>434300</v>
+      </c>
+      <c r="Q28">
+        <v>25.584081730000001</v>
+      </c>
+      <c r="R28">
+        <v>13.327005290000001</v>
+      </c>
+      <c r="S28">
+        <v>20.568435210000001</v>
+      </c>
+      <c r="T28">
+        <v>25.335536309999998</v>
+      </c>
+      <c r="U28">
+        <v>15.184941459999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>436</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>461.6</v>
+      </c>
+      <c r="D29">
+        <v>24.324324300000001</v>
+      </c>
+      <c r="E29">
+        <v>33.5907336</v>
+      </c>
+      <c r="F29">
+        <v>4.7762475999999996</v>
+      </c>
+      <c r="G29">
+        <v>8.064705193</v>
+      </c>
+      <c r="H29">
+        <v>13.534349840000001</v>
+      </c>
+      <c r="I29">
+        <v>61.104749200000001</v>
+      </c>
+      <c r="J29">
+        <v>11.455957010000001</v>
+      </c>
+      <c r="K29">
+        <v>67.3</v>
+      </c>
+      <c r="L29">
+        <v>42527.258405499997</v>
+      </c>
+      <c r="M29">
+        <v>4.9261704149999996</v>
+      </c>
+      <c r="N29">
+        <v>118150</v>
+      </c>
+      <c r="O29">
+        <v>103924.46153850001</v>
+      </c>
+      <c r="P29">
+        <v>259000</v>
+      </c>
+      <c r="Q29">
+        <v>24.450285869999998</v>
+      </c>
+      <c r="R29">
+        <v>17.282746889999999</v>
+      </c>
+      <c r="S29">
+        <v>20.322457350000001</v>
+      </c>
+      <c r="T29">
+        <v>24.009188550000001</v>
+      </c>
+      <c r="U29">
+        <v>13.935321330000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>437</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>489.3</v>
+      </c>
+      <c r="D30">
+        <v>26.5486726</v>
+      </c>
+      <c r="E30">
+        <v>44.616519199999999</v>
+      </c>
+      <c r="F30">
+        <v>3.7059761999999998</v>
+      </c>
+      <c r="G30">
+        <v>4.5953664529999996</v>
+      </c>
+      <c r="H30">
+        <v>10.03222407</v>
+      </c>
+      <c r="I30">
+        <v>61.827456130000002</v>
+      </c>
+      <c r="J30">
+        <v>16.017349070000002</v>
+      </c>
+      <c r="K30">
+        <v>73.8</v>
+      </c>
+      <c r="L30">
+        <v>53569.787159899999</v>
+      </c>
+      <c r="M30">
+        <v>7.7975923390000004</v>
+      </c>
+      <c r="N30">
+        <v>60320</v>
+      </c>
+      <c r="O30">
+        <v>184531.58223160001</v>
+      </c>
+      <c r="P30">
+        <v>135600</v>
+      </c>
+      <c r="Q30">
+        <v>24.791579200000001</v>
+      </c>
+      <c r="R30">
+        <v>15.3234271</v>
+      </c>
+      <c r="S30">
+        <v>21.375877169999999</v>
+      </c>
+      <c r="T30">
+        <v>23.642265940000001</v>
+      </c>
+      <c r="U30">
+        <v>14.866850599999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>438</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>526.1</v>
+      </c>
+      <c r="D31">
+        <v>35.977263899999997</v>
+      </c>
+      <c r="E31">
+        <v>55.7421522</v>
+      </c>
+      <c r="F31">
+        <v>5.5873625000000002</v>
+      </c>
+      <c r="G31">
+        <v>1.7557885849999999</v>
+      </c>
+      <c r="H31">
+        <v>17.308184950000001</v>
+      </c>
+      <c r="I31">
+        <v>60.943345770000001</v>
+      </c>
+      <c r="J31">
+        <v>11.29988036</v>
+      </c>
+      <c r="K31">
+        <v>73.3</v>
+      </c>
+      <c r="L31">
+        <v>48546.238808200003</v>
+      </c>
+      <c r="M31">
+        <v>7.0254951400000003</v>
+      </c>
+      <c r="N31">
+        <v>339520</v>
+      </c>
+      <c r="O31">
+        <v>186206.5334014</v>
+      </c>
+      <c r="P31">
+        <v>774100</v>
+      </c>
+      <c r="Q31">
+        <v>24.142464589999999</v>
+      </c>
+      <c r="R31">
+        <v>17.52982428</v>
+      </c>
+      <c r="S31">
+        <v>20.727226760000001</v>
+      </c>
+      <c r="T31">
+        <v>23.0162944</v>
+      </c>
+      <c r="U31">
+        <v>14.584189970000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>439</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>471.1</v>
+      </c>
+      <c r="D32">
+        <v>37.886441699999999</v>
+      </c>
+      <c r="E32">
+        <v>55.3647201</v>
+      </c>
+      <c r="F32">
+        <v>5.0997189000000001</v>
+      </c>
+      <c r="G32">
+        <v>3.3369625159999998</v>
+      </c>
+      <c r="H32">
+        <v>11.92257116</v>
+      </c>
+      <c r="I32">
+        <v>63.678482719999998</v>
+      </c>
+      <c r="J32">
+        <v>12.8854828</v>
+      </c>
+      <c r="K32">
+        <v>67.7</v>
+      </c>
+      <c r="L32">
+        <v>46313.232244300001</v>
+      </c>
+      <c r="M32">
+        <v>7.6373109929999998</v>
+      </c>
+      <c r="N32">
+        <v>194750</v>
+      </c>
+      <c r="O32">
+        <v>178284.43209369999</v>
+      </c>
+      <c r="P32">
+        <v>495000</v>
+      </c>
+      <c r="Q32">
+        <v>26.258740970000002</v>
+      </c>
+      <c r="R32">
+        <v>16.973104070000002</v>
+      </c>
+      <c r="S32">
+        <v>20.242788440000002</v>
+      </c>
+      <c r="T32">
+        <v>22.986139470000001</v>
+      </c>
+      <c r="U32">
+        <v>13.53922704</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>440</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>503.8</v>
+      </c>
+      <c r="D33">
+        <v>30.441035500000002</v>
+      </c>
+      <c r="E33">
+        <v>48.258229499999999</v>
+      </c>
+      <c r="F33">
+        <v>4.8522689000000003</v>
+      </c>
+      <c r="G33">
+        <v>1.9092524420000001</v>
+      </c>
+      <c r="H33">
+        <v>22.92922372</v>
+      </c>
+      <c r="I33">
+        <v>57.053046399999999</v>
+      </c>
+      <c r="J33">
+        <v>11.443126960000001</v>
+      </c>
+      <c r="K33">
+        <v>63.9</v>
+      </c>
+      <c r="L33">
+        <v>48126.242731099999</v>
+      </c>
+      <c r="M33">
+        <v>5.4132552939999998</v>
+      </c>
+      <c r="N33">
+        <v>282790</v>
+      </c>
+      <c r="O33">
+        <v>131046.3592105</v>
+      </c>
+      <c r="P33">
+        <v>625800</v>
+      </c>
+      <c r="Q33">
+        <v>23.516922860000001</v>
+      </c>
+      <c r="R33">
+        <v>17.91206386</v>
+      </c>
+      <c r="S33">
+        <v>19.497377140000001</v>
+      </c>
+      <c r="T33">
+        <v>24.623392150000001</v>
+      </c>
+      <c r="U33">
+        <v>14.450243990000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>441</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>696.8</v>
+      </c>
+      <c r="D34">
+        <v>64.202708200000004</v>
+      </c>
+      <c r="E34">
+        <v>112.3635812</v>
+      </c>
+      <c r="F34">
+        <v>4.3977272999999997</v>
+      </c>
+      <c r="G34">
+        <v>3.6207547529999999</v>
+      </c>
+      <c r="H34">
+        <v>44.633302450000002</v>
+      </c>
+      <c r="I34">
+        <v>33.549052090000004</v>
+      </c>
+      <c r="J34">
+        <v>8.0115653259999995</v>
+      </c>
+      <c r="K34">
+        <v>73.7</v>
+      </c>
+      <c r="L34">
+        <v>73590.342977499997</v>
+      </c>
+      <c r="M34">
+        <v>16.651741789999999</v>
+      </c>
+      <c r="N34">
+        <v>3960310</v>
+      </c>
+      <c r="O34">
+        <v>561436.59686070005</v>
+      </c>
+      <c r="P34">
+        <v>9896000</v>
+      </c>
+      <c r="Q34">
+        <v>24.509707039999999</v>
+      </c>
+      <c r="R34">
+        <v>17.137243529999999</v>
+      </c>
+      <c r="S34">
+        <v>24.885066949999999</v>
+      </c>
+      <c r="T34">
+        <v>21.766596870000001</v>
+      </c>
+      <c r="U34">
+        <v>11.701385610000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>442</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>527.6</v>
+      </c>
+      <c r="D35">
+        <v>34.0009315</v>
+      </c>
+      <c r="E35">
+        <v>66.3716814</v>
+      </c>
+      <c r="F35">
+        <v>3.7000321999999999</v>
+      </c>
+      <c r="G35">
+        <v>1.2881021509999999</v>
+      </c>
+      <c r="H35">
+        <v>13.3720474</v>
+      </c>
+      <c r="I35">
+        <v>65.118104059999993</v>
+      </c>
+      <c r="J35">
+        <v>12.624297929999999</v>
+      </c>
+      <c r="K35">
+        <v>68.5</v>
+      </c>
+      <c r="L35">
+        <v>55226.646178900002</v>
+      </c>
+      <c r="M35">
+        <v>9.1206242290000006</v>
+      </c>
+      <c r="N35">
+        <v>77100</v>
+      </c>
+      <c r="O35">
+        <v>224900.00048379999</v>
+      </c>
+      <c r="P35">
+        <v>214700</v>
+      </c>
+      <c r="Q35">
+        <v>28.338935339999999</v>
+      </c>
+      <c r="R35">
+        <v>17.437414189999998</v>
+      </c>
+      <c r="S35">
+        <v>21.617019599999999</v>
+      </c>
+      <c r="T35">
+        <v>20.854228079999999</v>
+      </c>
+      <c r="U35">
+        <v>11.75240279</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>443</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>500</v>
+      </c>
+      <c r="D36">
+        <v>41.822439500000002</v>
+      </c>
+      <c r="E36">
+        <v>59.919477399999998</v>
+      </c>
+      <c r="F36">
+        <v>4.9837395000000004</v>
+      </c>
+      <c r="G36">
+        <v>2.133491238</v>
+      </c>
+      <c r="H36">
+        <v>15.251183579999999</v>
+      </c>
+      <c r="I36">
+        <v>63.861238409999999</v>
+      </c>
+      <c r="J36">
+        <v>10.10421899</v>
+      </c>
+      <c r="K36">
+        <v>69.7</v>
+      </c>
+      <c r="L36">
+        <v>48351.931475899997</v>
+      </c>
+      <c r="M36">
+        <v>7.001092055</v>
+      </c>
+      <c r="N36">
+        <v>1046030</v>
+      </c>
+      <c r="O36">
+        <v>175419.96059659999</v>
+      </c>
+      <c r="P36">
+        <v>2434100</v>
+      </c>
+      <c r="Q36">
+        <v>25.408015209999999</v>
+      </c>
+      <c r="R36">
+        <v>15.450215439999999</v>
+      </c>
+      <c r="S36">
+        <v>20.88947379</v>
+      </c>
+      <c r="T36">
+        <v>23.954371819999999</v>
+      </c>
+      <c r="U36">
+        <v>14.29792374</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>444</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>455.9</v>
+      </c>
+      <c r="D37">
+        <v>20.634231100000001</v>
+      </c>
+      <c r="E37">
+        <v>33.231972200000001</v>
+      </c>
+      <c r="F37">
+        <v>5.4865485999999999</v>
+      </c>
+      <c r="G37">
+        <v>1.7136464890000001</v>
+      </c>
+      <c r="H37">
+        <v>7.6308861390000002</v>
+      </c>
+      <c r="I37">
+        <v>73.717658180000001</v>
+      </c>
+      <c r="J37">
+        <v>9.0070108100000006</v>
+      </c>
+      <c r="K37">
+        <v>74.5</v>
+      </c>
+      <c r="L37">
+        <v>43460.865483100002</v>
+      </c>
+      <c r="M37">
+        <v>6.3255191030000004</v>
+      </c>
+      <c r="N37">
+        <v>102350</v>
+      </c>
+      <c r="O37">
+        <v>135739.5894466</v>
+      </c>
+      <c r="P37">
+        <v>230100</v>
+      </c>
+      <c r="Q37">
+        <v>23.602112850000001</v>
+      </c>
+      <c r="R37">
+        <v>12.27211638</v>
+      </c>
+      <c r="S37">
+        <v>20.02920125</v>
+      </c>
+      <c r="T37">
+        <v>27.04732478</v>
+      </c>
+      <c r="U37">
+        <v>17.049244739999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>445</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>453.8</v>
+      </c>
+      <c r="D38">
+        <v>26.831345800000001</v>
+      </c>
+      <c r="E38">
+        <v>40.566439500000001</v>
+      </c>
+      <c r="F38">
+        <v>26.2165806</v>
+      </c>
+      <c r="G38">
+        <v>1.991182842</v>
+      </c>
+      <c r="H38">
+        <v>8.2702514350000005</v>
+      </c>
+      <c r="I38">
+        <v>72.012342000000004</v>
+      </c>
+      <c r="J38">
+        <v>9.6983683710000008</v>
+      </c>
+      <c r="K38">
+        <v>68.900000000000006</v>
+      </c>
+      <c r="L38">
+        <v>44886.325706700001</v>
+      </c>
+      <c r="M38">
+        <v>5.9744139819999997</v>
+      </c>
+      <c r="N38">
+        <v>208310</v>
+      </c>
+      <c r="O38">
+        <v>138755.67282380001</v>
+      </c>
+      <c r="P38">
+        <v>469600</v>
+      </c>
+      <c r="Q38">
+        <v>24.745539010000002</v>
+      </c>
+      <c r="R38">
+        <v>13.419633320000001</v>
+      </c>
+      <c r="S38">
+        <v>18.71650627</v>
+      </c>
+      <c r="T38">
+        <v>26.589051139999999</v>
+      </c>
+      <c r="U38">
+        <v>16.529270270000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>446</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>626.29999999999995</v>
+      </c>
+      <c r="D39">
+        <v>47.3644003</v>
+      </c>
+      <c r="E39">
+        <v>84.988540900000004</v>
+      </c>
+      <c r="F39">
+        <v>5.9853326999999998</v>
+      </c>
+      <c r="G39">
+        <v>2.8164935870000001</v>
+      </c>
+      <c r="H39">
+        <v>9.8291635040000003</v>
+      </c>
+      <c r="I39">
+        <v>70.016355849999997</v>
+      </c>
+      <c r="J39">
+        <v>7.1347518839999999</v>
+      </c>
+      <c r="K39">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="L39">
+        <v>64784.557418600001</v>
+      </c>
+      <c r="M39">
+        <v>8.9979761749999998</v>
+      </c>
+      <c r="N39">
+        <v>107550</v>
+      </c>
+      <c r="O39">
+        <v>265857.80324959999</v>
+      </c>
+      <c r="P39">
+        <v>261800</v>
+      </c>
+      <c r="Q39">
+        <v>26.88720004</v>
+      </c>
+      <c r="R39">
+        <v>13.52458193</v>
+      </c>
+      <c r="S39">
+        <v>23.93206361</v>
+      </c>
+      <c r="T39">
+        <v>24.599611769999999</v>
+      </c>
+      <c r="U39">
+        <v>11.05654266</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>447</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>491.8</v>
+      </c>
+      <c r="D40">
+        <v>28.280676799999998</v>
+      </c>
+      <c r="E40">
+        <v>38.989468700000003</v>
+      </c>
+      <c r="F40">
+        <v>4.9848673999999997</v>
+      </c>
+      <c r="G40">
+        <v>2.226106599</v>
+      </c>
+      <c r="H40">
+        <v>21.45323509</v>
+      </c>
+      <c r="I40">
+        <v>58.698972730000001</v>
+      </c>
+      <c r="J40">
+        <v>9.8359597700000005</v>
+      </c>
+      <c r="K40">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="L40">
+        <v>44536.767760700001</v>
+      </c>
+      <c r="M40">
+        <v>6.5651255610000003</v>
+      </c>
+      <c r="N40">
+        <v>383580</v>
+      </c>
+      <c r="O40">
+        <v>161178.05740359999</v>
+      </c>
+      <c r="P40">
+        <v>845000</v>
+      </c>
+      <c r="Q40">
+        <v>23.018163099999999</v>
+      </c>
+      <c r="R40">
+        <v>15.288447509999999</v>
+      </c>
+      <c r="S40">
+        <v>19.475979689999999</v>
+      </c>
+      <c r="T40">
+        <v>25.804907400000001</v>
+      </c>
+      <c r="U40">
+        <v>16.412502310000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>448</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>464.5</v>
+      </c>
+      <c r="D41">
+        <v>26.0851419</v>
+      </c>
+      <c r="E41">
+        <v>38.397328899999998</v>
+      </c>
+      <c r="F41">
+        <v>7.4608352</v>
+      </c>
+      <c r="G41">
+        <v>1.191374715</v>
+      </c>
+      <c r="H41">
+        <v>8.38452646</v>
+      </c>
+      <c r="I41">
+        <v>74.687825430000004</v>
+      </c>
+      <c r="J41">
+        <v>8.3510877150000002</v>
+      </c>
+      <c r="K41">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="L41">
+        <v>45594.876644800002</v>
+      </c>
+      <c r="M41">
+        <v>6.457228604</v>
+      </c>
+      <c r="N41">
+        <v>106155</v>
+      </c>
+      <c r="O41">
+        <v>156965.5348576</v>
+      </c>
+      <c r="P41">
+        <v>239600</v>
+      </c>
+      <c r="Q41">
+        <v>25.12341065</v>
+      </c>
+      <c r="R41">
+        <v>12.925497549999999</v>
+      </c>
+      <c r="S41">
+        <v>19.225458280000002</v>
+      </c>
+      <c r="T41">
+        <v>25.783430670000001</v>
+      </c>
+      <c r="U41">
+        <v>16.942202850000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>449</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>488.4</v>
+      </c>
+      <c r="D42">
+        <v>54.157303400000004</v>
+      </c>
+      <c r="E42">
+        <v>100.4494382</v>
+      </c>
+      <c r="F42">
+        <v>4.7127837000000001</v>
+      </c>
+      <c r="G42">
+        <v>2.5582440630000001</v>
+      </c>
+      <c r="H42">
+        <v>8.5446475389999996</v>
+      </c>
+      <c r="I42">
+        <v>70.251516969999997</v>
+      </c>
+      <c r="J42">
+        <v>10.34908982</v>
+      </c>
+      <c r="K42">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="L42">
+        <v>49058.9029094</v>
+      </c>
+      <c r="M42">
+        <v>7.4228306689999997</v>
+      </c>
+      <c r="N42">
+        <v>94090</v>
+      </c>
+      <c r="O42">
+        <v>195348.11927920001</v>
+      </c>
+      <c r="P42">
+        <v>222500</v>
+      </c>
+      <c r="Q42">
+        <v>25.38796335</v>
+      </c>
+      <c r="R42">
+        <v>15.22853411</v>
+      </c>
+      <c r="S42">
+        <v>22.19560615</v>
+      </c>
+      <c r="T42">
+        <v>23.883264409999999</v>
+      </c>
+      <c r="U42">
+        <v>13.30463198</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>450</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>436.8</v>
+      </c>
+      <c r="D43">
+        <v>33.709981200000001</v>
+      </c>
+      <c r="E43">
+        <v>42.561205299999997</v>
+      </c>
+      <c r="F43">
+        <v>5.5184986</v>
+      </c>
+      <c r="G43">
+        <v>6.3356592589999998</v>
+      </c>
+      <c r="H43">
+        <v>7.8062356309999998</v>
+      </c>
+      <c r="I43">
+        <v>61.727907070000001</v>
+      </c>
+      <c r="J43">
+        <v>14.2193361</v>
+      </c>
+      <c r="K43">
+        <v>79.2</v>
+      </c>
+      <c r="L43">
+        <v>48881.066997900001</v>
+      </c>
+      <c r="M43">
+        <v>9.5910601030000002</v>
+      </c>
+      <c r="N43">
+        <v>120550</v>
+      </c>
+      <c r="O43">
+        <v>224807.21028570001</v>
+      </c>
+      <c r="P43">
+        <v>265500</v>
+      </c>
+      <c r="Q43">
+        <v>21.734108989999999</v>
+      </c>
+      <c r="R43">
+        <v>15.13077563</v>
+      </c>
+      <c r="S43">
+        <v>19.93249286</v>
+      </c>
+      <c r="T43">
+        <v>24.863313600000001</v>
+      </c>
+      <c r="U43">
+        <v>18.33930891</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>451</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>469.3</v>
+      </c>
+      <c r="D44">
+        <v>29.851874200000001</v>
+      </c>
+      <c r="E44">
+        <v>41.414752100000001</v>
+      </c>
+      <c r="F44">
+        <v>4.9414663000000001</v>
+      </c>
+      <c r="G44">
+        <v>3.2720706150000001</v>
+      </c>
+      <c r="H44">
+        <v>16.338739140000001</v>
+      </c>
+      <c r="I44">
+        <v>60.412338069999997</v>
+      </c>
+      <c r="J44">
+        <v>11.413202630000001</v>
+      </c>
+      <c r="K44">
+        <v>72</v>
+      </c>
+      <c r="L44">
+        <v>44326.8490657</v>
+      </c>
+      <c r="M44">
+        <v>6.4315407850000001</v>
+      </c>
+      <c r="N44">
+        <v>286350</v>
+      </c>
+      <c r="O44">
+        <v>161841.37321290001</v>
+      </c>
+      <c r="P44">
+        <v>661600</v>
+      </c>
+      <c r="Q44">
+        <v>24.1222177</v>
+      </c>
+      <c r="R44">
+        <v>16.803138619999999</v>
+      </c>
+      <c r="S44">
+        <v>20.14338528</v>
+      </c>
+      <c r="T44">
+        <v>23.84646476</v>
+      </c>
+      <c r="U44">
+        <v>15.084793639999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>452</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>575.5</v>
+      </c>
+      <c r="D45">
+        <v>30.075188000000001</v>
+      </c>
+      <c r="E45">
+        <v>42.919799500000003</v>
+      </c>
+      <c r="F45">
+        <v>4.7908869999999997</v>
+      </c>
+      <c r="G45">
+        <v>17.06848883</v>
+      </c>
+      <c r="H45">
+        <v>18.561175810000002</v>
+      </c>
+      <c r="I45">
+        <v>36.622401760000002</v>
+      </c>
+      <c r="J45">
+        <v>16.810635040000001</v>
+      </c>
+      <c r="K45">
+        <v>74.5</v>
+      </c>
+      <c r="L45">
+        <v>60161.350173899998</v>
+      </c>
+      <c r="M45">
+        <v>16.728243469999999</v>
+      </c>
+      <c r="N45">
+        <v>58030</v>
+      </c>
+      <c r="O45">
+        <v>491910.72742469999</v>
+      </c>
+      <c r="P45">
+        <v>159600</v>
+      </c>
+      <c r="Q45">
+        <v>24.148486559999998</v>
+      </c>
+      <c r="R45">
+        <v>26.101668140000001</v>
+      </c>
+      <c r="S45">
+        <v>20.631179809999999</v>
+      </c>
+      <c r="T45">
+        <v>18.1645228</v>
+      </c>
+      <c r="U45">
+        <v>10.954142689999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>453</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>511.1</v>
+      </c>
+      <c r="D46">
+        <v>34.536082499999999</v>
+      </c>
+      <c r="E46">
+        <v>60.309278399999997</v>
+      </c>
+      <c r="F46">
+        <v>5.7301824999999997</v>
+      </c>
+      <c r="G46">
+        <v>5.6676207349999999</v>
+      </c>
+      <c r="H46">
+        <v>9.7746581250000002</v>
+      </c>
+      <c r="I46">
+        <v>67.414020260000001</v>
+      </c>
+      <c r="J46">
+        <v>8.5252828130000005</v>
+      </c>
+      <c r="K46">
+        <v>75.5</v>
+      </c>
+      <c r="L46">
+        <v>50246.470983599997</v>
+      </c>
+      <c r="M46">
+        <v>7.2883019349999998</v>
+      </c>
+      <c r="N46">
+        <v>80480</v>
+      </c>
+      <c r="O46">
+        <v>182825.59639019999</v>
+      </c>
+      <c r="P46">
+        <v>194000</v>
+      </c>
+      <c r="Q46">
+        <v>26.23467715</v>
+      </c>
+      <c r="R46">
+        <v>15.00182431</v>
+      </c>
+      <c r="S46">
+        <v>21.954354110000001</v>
+      </c>
+      <c r="T46">
+        <v>23.261322979999999</v>
+      </c>
+      <c r="U46">
+        <v>13.547821450000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>454</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>458.3</v>
+      </c>
+      <c r="D47">
+        <v>29.691663500000001</v>
+      </c>
+      <c r="E47">
+        <v>33.307955800000002</v>
+      </c>
+      <c r="F47">
+        <v>4.0350869999999999</v>
+      </c>
+      <c r="G47">
+        <v>2.6007525579999999</v>
+      </c>
+      <c r="H47">
+        <v>11.66124666</v>
+      </c>
+      <c r="I47">
+        <v>64.028740229999997</v>
+      </c>
+      <c r="J47">
+        <v>14.12493828</v>
+      </c>
+      <c r="K47">
+        <v>74</v>
+      </c>
+      <c r="L47">
+        <v>47124.172921799996</v>
+      </c>
+      <c r="M47">
+        <v>8.1252657950000007</v>
+      </c>
+      <c r="N47">
+        <v>115560</v>
+      </c>
+      <c r="O47">
+        <v>179948.63649899999</v>
+      </c>
+      <c r="P47">
+        <v>262700</v>
+      </c>
+      <c r="Q47">
+        <v>23.297865699999999</v>
+      </c>
+      <c r="R47">
+        <v>16.861816650000002</v>
+      </c>
+      <c r="S47">
+        <v>18.980123559999999</v>
+      </c>
+      <c r="T47">
+        <v>24.589677980000001</v>
+      </c>
+      <c r="U47">
+        <v>16.270516099999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>455</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>517.4</v>
+      </c>
+      <c r="D48">
+        <v>32.852864099999998</v>
+      </c>
+      <c r="E48">
+        <v>47.454137000000003</v>
+      </c>
+      <c r="F48">
+        <v>4.1534662999999998</v>
+      </c>
+      <c r="G48">
+        <v>6.022953008</v>
+      </c>
+      <c r="H48">
+        <v>8.2386340790000006</v>
+      </c>
+      <c r="I48">
+        <v>65.790447240000006</v>
+      </c>
+      <c r="J48">
+        <v>10.90710224</v>
+      </c>
+      <c r="K48">
+        <v>74.3</v>
+      </c>
+      <c r="L48">
+        <v>54378.6971586</v>
+      </c>
+      <c r="M48">
+        <v>8.8592370460000005</v>
+      </c>
+      <c r="N48">
+        <v>229250</v>
+      </c>
+      <c r="O48">
+        <v>234074.1101389</v>
+      </c>
+      <c r="P48">
+        <v>534200</v>
+      </c>
+      <c r="Q48">
+        <v>23.911274890000001</v>
+      </c>
+      <c r="R48">
+        <v>14.3371485</v>
+      </c>
+      <c r="S48">
+        <v>19.212490599999999</v>
+      </c>
+      <c r="T48">
+        <v>25.2835407</v>
+      </c>
+      <c r="U48">
+        <v>17.25554532</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>456</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>459.4</v>
+      </c>
+      <c r="D49">
+        <v>36.675824200000001</v>
+      </c>
+      <c r="E49">
+        <v>46.0164835</v>
+      </c>
+      <c r="F49">
+        <v>6.2875908999999996</v>
+      </c>
+      <c r="G49">
+        <v>2.1866703520000002</v>
+      </c>
+      <c r="H49">
+        <v>8.3233991580000009</v>
+      </c>
+      <c r="I49">
+        <v>70.72902449</v>
+      </c>
+      <c r="J49">
+        <v>9.4239330120000009</v>
+      </c>
+      <c r="K49">
+        <v>76.7</v>
+      </c>
+      <c r="L49">
+        <v>47826.469810100003</v>
+      </c>
+      <c r="M49">
+        <v>6.2719551789999999</v>
+      </c>
+      <c r="N49">
+        <v>159290</v>
+      </c>
+      <c r="O49">
+        <v>163478.5117417</v>
+      </c>
+      <c r="P49">
+        <v>363900</v>
+      </c>
+      <c r="Q49">
+        <v>23.870835599999999</v>
+      </c>
+      <c r="R49">
+        <v>13.967745369999999</v>
+      </c>
+      <c r="S49">
+        <v>20.287923589999998</v>
+      </c>
+      <c r="T49">
+        <v>25.987475239999998</v>
+      </c>
+      <c r="U49">
+        <v>15.88602019</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>457</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>634.4</v>
+      </c>
+      <c r="D50">
+        <v>46.2589258</v>
+      </c>
+      <c r="E50">
+        <v>75.4424092</v>
+      </c>
+      <c r="F50">
+        <v>4.9316690999999997</v>
+      </c>
+      <c r="G50">
+        <v>3.222125052</v>
+      </c>
+      <c r="H50">
+        <v>15.267104550000001</v>
+      </c>
+      <c r="I50">
+        <v>59.179800159999999</v>
+      </c>
+      <c r="J50">
+        <v>10.88079688</v>
+      </c>
+      <c r="K50">
+        <v>77.400000000000006</v>
+      </c>
+      <c r="L50">
+        <v>71591.811379199993</v>
+      </c>
+      <c r="M50">
+        <v>11.25649531</v>
+      </c>
+      <c r="N50">
+        <v>131400</v>
+      </c>
+      <c r="O50">
+        <v>375229.99847679998</v>
+      </c>
+      <c r="P50">
+        <v>322100</v>
+      </c>
+      <c r="Q50">
+        <v>24.857938969999999</v>
+      </c>
+      <c r="R50">
+        <v>14.57246241</v>
+      </c>
+      <c r="S50">
+        <v>23.299621389999999</v>
+      </c>
+      <c r="T50">
+        <v>23.84722554</v>
+      </c>
+      <c r="U50">
+        <v>13.42275169</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>458</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>465.8</v>
+      </c>
+      <c r="D51">
+        <v>29.199277500000001</v>
+      </c>
+      <c r="E51">
+        <v>40.8789886</v>
+      </c>
+      <c r="F51">
+        <v>5.4478532</v>
+      </c>
+      <c r="G51">
+        <v>1.4627396720000001</v>
+      </c>
+      <c r="H51">
+        <v>16.048375650000001</v>
+      </c>
+      <c r="I51">
+        <v>63.933750760000002</v>
+      </c>
+      <c r="J51">
+        <v>10.532059719999999</v>
+      </c>
+      <c r="K51">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="L51">
+        <v>44050.477884300002</v>
+      </c>
+      <c r="M51">
+        <v>6.8054288139999999</v>
+      </c>
+      <c r="N51">
+        <v>355010</v>
+      </c>
+      <c r="O51">
+        <v>161231.56599929999</v>
+      </c>
+      <c r="P51">
+        <v>830500</v>
+      </c>
+      <c r="Q51">
+        <v>24.578445339999998</v>
+      </c>
+      <c r="R51">
+        <v>15.505112479999999</v>
+      </c>
+      <c r="S51">
+        <v>19.77103082</v>
+      </c>
+      <c r="T51">
+        <v>24.028924239999998</v>
+      </c>
+      <c r="U51">
+        <v>16.116487110000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>459</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>587.6</v>
+      </c>
+      <c r="D52">
+        <v>41.180507900000002</v>
+      </c>
+      <c r="E52">
+        <v>86.479066599999996</v>
+      </c>
+      <c r="F52">
+        <v>5.2424474999999999</v>
+      </c>
+      <c r="G52">
+        <v>2.326894502</v>
+      </c>
+      <c r="H52">
+        <v>15.068350669999999</v>
+      </c>
+      <c r="I52">
+        <v>65.552748890000004</v>
+      </c>
+      <c r="J52">
+        <v>9.1664190189999992</v>
+      </c>
+      <c r="K52">
+        <v>74.3</v>
+      </c>
+      <c r="L52">
+        <v>71592.205047900003</v>
+      </c>
+      <c r="M52">
+        <v>10.257894909999999</v>
+      </c>
+      <c r="N52">
+        <v>53080</v>
+      </c>
+      <c r="O52">
+        <v>290548.71861470002</v>
+      </c>
+      <c r="P52">
+        <v>145700</v>
+      </c>
+      <c r="Q52">
+        <v>28.799971469999999</v>
+      </c>
+      <c r="R52">
+        <v>16.35105738</v>
+      </c>
+      <c r="S52">
+        <v>25.606790060000002</v>
+      </c>
+      <c r="T52">
+        <v>20.095574339999999</v>
+      </c>
+      <c r="U52">
+        <v>9.1466067540000004</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>460</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>555.6</v>
+      </c>
+      <c r="D53">
+        <v>38.0449141</v>
+      </c>
+      <c r="E53">
+        <v>58.388375199999999</v>
+      </c>
+      <c r="F53">
+        <v>4.1894169000000003</v>
+      </c>
+      <c r="G53">
+        <v>3.8026416109999999</v>
+      </c>
+      <c r="H53">
+        <v>10.054603759999999</v>
+      </c>
+      <c r="I53">
+        <v>65.182535770000001</v>
+      </c>
+      <c r="J53">
+        <v>12.555500739999999</v>
+      </c>
+      <c r="K53">
+        <v>76.2</v>
+      </c>
+      <c r="L53">
+        <v>52460.699011199998</v>
+      </c>
+      <c r="M53">
+        <v>9.483148881</v>
+      </c>
+      <c r="N53">
+        <v>158260</v>
+      </c>
+      <c r="O53">
+        <v>235529.3757602</v>
+      </c>
+      <c r="P53">
+        <v>378600</v>
+      </c>
+      <c r="Q53">
+        <v>23.86123547</v>
+      </c>
+      <c r="R53">
+        <v>18.154225159999999</v>
+      </c>
+      <c r="S53">
+        <v>20.639580649999999</v>
+      </c>
+      <c r="T53">
+        <v>23.09207056</v>
+      </c>
+      <c r="U53">
+        <v>14.25288817</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>461</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>405</v>
+      </c>
+      <c r="D54">
+        <v>44.475920700000003</v>
+      </c>
+      <c r="E54">
+        <v>61.614730899999998</v>
+      </c>
+      <c r="F54">
+        <v>3.726483</v>
+      </c>
+      <c r="G54">
+        <v>2.0734930619999998</v>
+      </c>
+      <c r="H54">
+        <v>19.538802279999999</v>
+      </c>
+      <c r="I54">
+        <v>59.510902819999998</v>
+      </c>
+      <c r="J54">
+        <v>9.2019284890000002</v>
+      </c>
+      <c r="K54">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="L54">
+        <v>51356.036484600001</v>
+      </c>
+      <c r="M54">
+        <v>9.9512906169999997</v>
+      </c>
+      <c r="N54">
+        <v>152850</v>
+      </c>
+      <c r="O54">
+        <v>282946.45098810003</v>
+      </c>
+      <c r="P54">
+        <v>353000</v>
+      </c>
+      <c r="Q54">
+        <v>22.997135870000001</v>
+      </c>
+      <c r="R54">
+        <v>10.99647491</v>
+      </c>
+      <c r="S54">
+        <v>19.890652719999999</v>
+      </c>
+      <c r="T54">
+        <v>26.844293189999998</v>
+      </c>
+      <c r="U54">
+        <v>19.271443309999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>462</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>441</v>
+      </c>
+      <c r="D55">
+        <v>26.2810354</v>
+      </c>
+      <c r="E55">
+        <v>36.714210199999997</v>
+      </c>
+      <c r="F55">
+        <v>5.9362791000000001</v>
+      </c>
+      <c r="G55">
+        <v>1.3548874449999999</v>
+      </c>
+      <c r="H55">
+        <v>7.4766581050000003</v>
+      </c>
+      <c r="I55">
+        <v>74.292793470000007</v>
+      </c>
+      <c r="J55">
+        <v>9.2974769599999991</v>
+      </c>
+      <c r="K55">
+        <v>72.3</v>
+      </c>
+      <c r="L55">
+        <v>42384.564707999998</v>
+      </c>
+      <c r="M55">
+        <v>5.6098343789999996</v>
+      </c>
+      <c r="N55">
+        <v>169100</v>
+      </c>
+      <c r="O55">
+        <v>125314.855438</v>
+      </c>
+      <c r="P55">
+        <v>378700</v>
+      </c>
+      <c r="Q55">
+        <v>24.073224830000001</v>
+      </c>
+      <c r="R55">
+        <v>14.40869558</v>
+      </c>
+      <c r="S55">
+        <v>19.58302827</v>
+      </c>
+      <c r="T55">
+        <v>25.48842922</v>
+      </c>
+      <c r="U55">
+        <v>16.446622090000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>463</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>476.3</v>
+      </c>
+      <c r="D56">
+        <v>19.119769099999999</v>
+      </c>
+      <c r="E56">
+        <v>30.6637807</v>
+      </c>
+      <c r="F56">
+        <v>5.371702</v>
+      </c>
+      <c r="G56">
+        <v>1.3068775669999999</v>
+      </c>
+      <c r="H56">
+        <v>15.477611080000001</v>
+      </c>
+      <c r="I56">
+        <v>66.844154029999999</v>
+      </c>
+      <c r="J56">
+        <v>9.3077992940000005</v>
+      </c>
+      <c r="K56">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="L56">
+        <v>47766.331595600001</v>
+      </c>
+      <c r="M56">
+        <v>5.1632665190000004</v>
+      </c>
+      <c r="N56">
+        <v>125220</v>
+      </c>
+      <c r="O56">
+        <v>123424.7881773</v>
+      </c>
+      <c r="P56">
+        <v>277200</v>
+      </c>
+      <c r="Q56">
+        <v>22.74106553</v>
+      </c>
+      <c r="R56">
+        <v>13.304247459999999</v>
+      </c>
+      <c r="S56">
+        <v>19.18433718</v>
+      </c>
+      <c r="T56">
+        <v>27.78596473</v>
+      </c>
+      <c r="U56">
+        <v>16.984385100000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>464</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>450.3</v>
+      </c>
+      <c r="D57">
+        <v>26.604068900000001</v>
+      </c>
+      <c r="E57">
+        <v>33.646322400000003</v>
+      </c>
+      <c r="F57">
+        <v>26.784960600000002</v>
+      </c>
+      <c r="G57">
+        <v>1.384656278</v>
+      </c>
+      <c r="H57">
+        <v>6.0146007060000004</v>
+      </c>
+      <c r="I57">
+        <v>75.481075329999996</v>
+      </c>
+      <c r="J57">
+        <v>8.9854302019999999</v>
+      </c>
+      <c r="K57">
+        <v>68.7</v>
+      </c>
+      <c r="L57">
+        <v>42787.815842399999</v>
+      </c>
+      <c r="M57">
+        <v>6.0293115139999998</v>
+      </c>
+      <c r="N57">
+        <v>175407</v>
+      </c>
+      <c r="O57">
+        <v>143670.77238430001</v>
+      </c>
+      <c r="P57">
+        <v>383400</v>
+      </c>
+      <c r="Q57">
+        <v>22.771655209999999</v>
+      </c>
+      <c r="R57">
+        <v>13.962015129999999</v>
+      </c>
+      <c r="S57">
+        <v>18.910871490000002</v>
+      </c>
+      <c r="T57">
+        <v>26.177887470000002</v>
+      </c>
+      <c r="U57">
+        <v>18.177570710000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>465</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>564.20000000000005</v>
+      </c>
+      <c r="D58">
+        <v>34.069981599999998</v>
+      </c>
+      <c r="E58">
+        <v>54.097605899999998</v>
+      </c>
+      <c r="F58">
+        <v>5.6981558999999997</v>
+      </c>
+      <c r="G58">
+        <v>4.1936456040000003</v>
+      </c>
+      <c r="H58">
+        <v>9.6868464549999995</v>
+      </c>
+      <c r="I58">
+        <v>68.162266320000001</v>
+      </c>
+      <c r="J58">
+        <v>9.4932373810000001</v>
+      </c>
+      <c r="K58">
+        <v>79</v>
+      </c>
+      <c r="L58">
+        <v>59212.391889999999</v>
+      </c>
+      <c r="M58">
+        <v>7.7017265000000004</v>
+      </c>
+      <c r="N58">
+        <v>93900</v>
+      </c>
+      <c r="O58">
+        <v>204650.2765562</v>
+      </c>
+      <c r="P58">
+        <v>217200</v>
+      </c>
+      <c r="Q58">
+        <v>24.485551449999999</v>
+      </c>
+      <c r="R58">
+        <v>13.35558148</v>
+      </c>
+      <c r="S58">
+        <v>23.110979360000002</v>
+      </c>
+      <c r="T58">
+        <v>25.252443150000001</v>
+      </c>
+      <c r="U58">
+        <v>13.795444549999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>466</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>487.1</v>
+      </c>
+      <c r="D59">
+        <v>27.161214999999999</v>
+      </c>
+      <c r="E59">
+        <v>37.0911215</v>
+      </c>
+      <c r="F59">
+        <v>6.3464891999999997</v>
+      </c>
+      <c r="G59">
+        <v>2.0976879500000001</v>
+      </c>
+      <c r="H59">
+        <v>5.3845761239999996</v>
+      </c>
+      <c r="I59">
+        <v>76.568162099999995</v>
+      </c>
+      <c r="J59">
+        <v>7.4516408920000003</v>
+      </c>
+      <c r="K59">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="L59">
+        <v>44042.769857400002</v>
+      </c>
+      <c r="M59">
+        <v>6.7069240389999996</v>
+      </c>
+      <c r="N59">
+        <v>71960</v>
+      </c>
+      <c r="O59">
+        <v>160255.2429862</v>
+      </c>
+      <c r="P59">
+        <v>171200</v>
+      </c>
+      <c r="Q59">
+        <v>26.068614570000001</v>
+      </c>
+      <c r="R59">
+        <v>13.052610100000001</v>
+      </c>
+      <c r="S59">
+        <v>20.600572490000001</v>
+      </c>
+      <c r="T59">
+        <v>25.822576680000001</v>
+      </c>
+      <c r="U59">
+        <v>14.45562617</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>467</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>463</v>
+      </c>
+      <c r="D60">
+        <v>27.561413999999999</v>
+      </c>
+      <c r="E60">
+        <v>43.888556000000001</v>
+      </c>
+      <c r="F60">
+        <v>6.4990315000000001</v>
+      </c>
+      <c r="G60">
+        <v>1.2309982349999999</v>
+      </c>
+      <c r="H60">
+        <v>9.6115341040000004</v>
+      </c>
+      <c r="I60">
+        <v>71.866849329999994</v>
+      </c>
+      <c r="J60">
+        <v>9.4666332959999995</v>
+      </c>
+      <c r="K60">
+        <v>71.3</v>
+      </c>
+      <c r="L60">
+        <v>44366.862557200002</v>
+      </c>
+      <c r="M60">
+        <v>6.3694175389999996</v>
+      </c>
+      <c r="N60">
+        <v>149690</v>
+      </c>
+      <c r="O60">
+        <v>145036.73289740001</v>
+      </c>
+      <c r="P60">
+        <v>333800</v>
+      </c>
+      <c r="Q60">
+        <v>23.318714570000001</v>
+      </c>
+      <c r="R60">
+        <v>12.38011644</v>
+      </c>
+      <c r="S60">
+        <v>20.044071120000002</v>
+      </c>
+      <c r="T60">
+        <v>27.333912349999999</v>
+      </c>
+      <c r="U60">
+        <v>16.923185520000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>468</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>513.79999999999995</v>
+      </c>
+      <c r="D61">
+        <v>37.072701000000002</v>
+      </c>
+      <c r="E61">
+        <v>59.220028900000003</v>
+      </c>
+      <c r="F61">
+        <v>6.7650907</v>
+      </c>
+      <c r="G61">
+        <v>2.5551281029999999</v>
+      </c>
+      <c r="H61">
+        <v>7.0952645360000002</v>
+      </c>
+      <c r="I61">
+        <v>73.733838340000005</v>
+      </c>
+      <c r="J61">
+        <v>6.9782660429999996</v>
+      </c>
+      <c r="K61">
+        <v>78.5</v>
+      </c>
+      <c r="L61">
+        <v>52456.716153100002</v>
+      </c>
+      <c r="M61">
+        <v>6.7552409210000004</v>
+      </c>
+      <c r="N61">
+        <v>90570</v>
+      </c>
+      <c r="O61">
+        <v>193164.76309620001</v>
+      </c>
+      <c r="P61">
+        <v>207700</v>
+      </c>
+      <c r="Q61">
+        <v>24.065411319999999</v>
+      </c>
+      <c r="R61">
+        <v>12.160037190000001</v>
+      </c>
+      <c r="S61">
+        <v>20.930336059999998</v>
+      </c>
+      <c r="T61">
+        <v>26.914670569999998</v>
+      </c>
+      <c r="U61">
+        <v>15.929544870000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>469</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>419.3</v>
+      </c>
+      <c r="D62">
+        <v>26.397515500000001</v>
+      </c>
+      <c r="E62">
+        <v>41.6149068</v>
+      </c>
+      <c r="F62">
+        <v>4.7685544999999996</v>
+      </c>
+      <c r="G62">
+        <v>1.5702964479999999</v>
+      </c>
+      <c r="H62">
+        <v>7.9168556710000004</v>
+      </c>
+      <c r="I62">
+        <v>74.026736400000004</v>
+      </c>
+      <c r="J62">
+        <v>8.8727753020000009</v>
+      </c>
+      <c r="K62">
+        <v>76.5</v>
+      </c>
+      <c r="L62">
+        <v>45396.9131624</v>
+      </c>
+      <c r="M62">
+        <v>5.4059390230000002</v>
+      </c>
+      <c r="N62">
+        <v>143220</v>
+      </c>
+      <c r="O62">
+        <v>128944.61995389999</v>
+      </c>
+      <c r="P62">
+        <v>322000</v>
+      </c>
+      <c r="Q62">
+        <v>23.773867469999999</v>
+      </c>
+      <c r="R62">
+        <v>12.42225082</v>
+      </c>
+      <c r="S62">
+        <v>20.799813749999998</v>
+      </c>
+      <c r="T62">
+        <v>26.754528090000001</v>
+      </c>
+      <c r="U62">
+        <v>16.24953988</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>470</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>436.9</v>
+      </c>
+      <c r="D63">
+        <v>38.997214499999998</v>
+      </c>
+      <c r="E63">
+        <v>47.818013000000001</v>
+      </c>
+      <c r="F63">
+        <v>3.8750833999999998</v>
+      </c>
+      <c r="G63">
+        <v>5.028551105</v>
+      </c>
+      <c r="H63">
+        <v>9.4268044500000006</v>
+      </c>
+      <c r="I63">
+        <v>61.138882850000002</v>
+      </c>
+      <c r="J63">
+        <v>13.58400348</v>
+      </c>
+      <c r="K63">
+        <v>80.5</v>
+      </c>
+      <c r="L63">
+        <v>54478.723279500002</v>
+      </c>
+      <c r="M63">
+        <v>10.691860999999999</v>
+      </c>
+      <c r="N63">
+        <v>49220</v>
+      </c>
+      <c r="O63">
+        <v>279100.33954329998</v>
+      </c>
+      <c r="P63">
+        <v>107700</v>
+      </c>
+      <c r="Q63">
+        <v>22.12155963</v>
+      </c>
+      <c r="R63">
+        <v>10.99961774</v>
+      </c>
+      <c r="S63">
+        <v>20.342125379999999</v>
+      </c>
+      <c r="T63">
+        <v>25.91934251</v>
+      </c>
+      <c r="U63">
+        <v>20.61735474</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>471</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>469.1</v>
+      </c>
+      <c r="D64">
+        <v>32.141131000000001</v>
+      </c>
+      <c r="E64">
+        <v>40.115998099999999</v>
+      </c>
+      <c r="F64">
+        <v>4.7147287000000002</v>
+      </c>
+      <c r="G64">
+        <v>11.24988604</v>
+      </c>
+      <c r="H64">
+        <v>9.6646103669999999</v>
+      </c>
+      <c r="I64">
+        <v>51.569574860000003</v>
+      </c>
+      <c r="J64">
+        <v>17.68316772</v>
+      </c>
+      <c r="K64">
+        <v>76.7</v>
+      </c>
+      <c r="L64">
+        <v>48259.772413500003</v>
+      </c>
+      <c r="M64">
+        <v>9.684350491</v>
+      </c>
+      <c r="N64">
+        <v>87210</v>
+      </c>
+      <c r="O64">
+        <v>246857.96775489999</v>
+      </c>
+      <c r="P64">
+        <v>206900</v>
+      </c>
+      <c r="Q64">
+        <v>22.132683</v>
+      </c>
+      <c r="R64">
+        <v>17.119327850000001</v>
+      </c>
+      <c r="S64">
+        <v>19.600002020000002</v>
+      </c>
+      <c r="T64">
+        <v>24.276070310000001</v>
+      </c>
+      <c r="U64">
+        <v>16.87191683</v>
       </c>
     </row>
   </sheetData>

</xml_diff>